<commit_message>
I was added to db
</commit_message>
<xml_diff>
--- a/DB.xlsx
+++ b/DB.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t xml:space="preserve">№</t>
   </si>
@@ -28,7 +28,7 @@
     <t xml:space="preserve">ID</t>
   </si>
   <si>
-    <t xml:space="preserve">Name</t>
+    <t xml:space="preserve">First Name</t>
   </si>
   <si>
     <t xml:space="preserve">Last Name</t>
@@ -62,6 +62,15 @@
   </si>
   <si>
     <t xml:space="preserve">Murat Akhmetov </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nurmukhanbet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rakhimbayev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nurmukhanbet Rakhimbayev </t>
   </si>
 </sst>
 </file>
@@ -72,11 +81,12 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -96,14 +106,9 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="JetBrains Mono"/>
+      <name val="Ubuntu"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -168,7 +173,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -196,7 +201,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -204,7 +209,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="3.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="23.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="34.18"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="1" width="11.52"/>
   </cols>
@@ -242,13 +247,13 @@
       <c r="B2" s="3" t="n">
         <v>830667168</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="4" t="n">
@@ -268,13 +273,13 @@
       <c r="B3" s="3" t="n">
         <v>294728712</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="4" t="n">
@@ -288,14 +293,30 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="A4" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>287100650</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>350</v>
+      </c>
+      <c r="G4" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2"/>
@@ -303,9 +324,9 @@
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2"/>
@@ -313,9 +334,9 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2"/>
@@ -323,9 +344,9 @@
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2"/>
@@ -333,9 +354,9 @@
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
@@ -343,9 +364,9 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2"/>
@@ -353,9 +374,9 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2"/>
@@ -363,9 +384,9 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2"/>
@@ -373,9 +394,9 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2"/>
@@ -383,9 +404,9 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2"/>
@@ -393,9 +414,9 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2"/>
@@ -403,9 +424,9 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2"/>
@@ -413,9 +434,9 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2"/>
@@ -423,9 +444,9 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2"/>
@@ -433,9 +454,9 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2"/>
@@ -443,9 +464,9 @@
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2"/>
@@ -453,9 +474,9 @@
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2"/>
@@ -463,9 +484,9 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2"/>
@@ -473,9 +494,9 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2"/>
@@ -483,9 +504,9 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>